<commit_message>
Update 20250123 - Add WL hydrograph
</commit_message>
<xml_diff>
--- a/CrystalSpringsLG/Rivercell_Fragment_Polygon-1.xlsx
+++ b/CrystalSpringsLG/Rivercell_Fragment_Polygon-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Eval_Permit\GEURINK\StrategicPlanning\MWP2023\CWF\Task5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Mac_xSSD/MWP-IHM/CrystalSpringsLG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D69B99-6C6B-4C62-A70F-0C56FF00C58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8760925-03A4-B045-B2E6-478E8C0765D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8278C831-B167-494D-BAB2-B994A46DB11F}"/>
+    <workbookView xWindow="47680" yWindow="2020" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8278C831-B167-494D-BAB2-B994A46DB11F}"/>
   </bookViews>
   <sheets>
     <sheet name="WaterbodyPolygons" sheetId="2" r:id="rId1"/>
@@ -167,11 +167,13 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -398,6 +400,50 @@
         <a:xfrm>
           <a:off x="2438400" y="190500"/>
           <a:ext cx="2142857" cy="2323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>334819</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>80543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DB4BB3E-E17F-B68C-14CE-F7BBE60CC0CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5357091" y="196273"/>
+          <a:ext cx="5022273" cy="6557543"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -777,18 +823,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32E2BD1-587B-4436-9304-897E286AED53}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -796,7 +842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L2" s="7" t="s">
         <v>11</v>
       </c>
@@ -806,7 +852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L3" s="4" t="s">
         <v>3</v>
       </c>
@@ -820,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L4" s="2">
         <v>406962</v>
       </c>
@@ -834,7 +880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L5" s="2">
         <v>406940</v>
       </c>
@@ -845,7 +891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L6" s="2">
         <v>406941</v>
       </c>
@@ -861,7 +907,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L7" s="2">
         <v>403631</v>
       </c>
@@ -875,7 +921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L8" s="2">
         <v>398947</v>
       </c>
@@ -889,7 +935,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L9" s="2">
         <v>400047</v>
       </c>
@@ -903,7 +949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L10" s="2">
         <v>399757</v>
       </c>
@@ -914,7 +960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L11" s="2">
         <v>398941</v>
       </c>
@@ -940,7 +986,7 @@
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L12" s="2">
         <v>398939</v>
       </c>
@@ -966,7 +1012,7 @@
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L13" s="2">
         <v>398943</v>
       </c>
@@ -977,7 +1023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L14" s="3">
         <v>398938</v>
       </c>
@@ -988,7 +1034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L15" s="2">
         <v>403628</v>
       </c>
@@ -999,7 +1045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="L16" s="2">
         <v>404982</v>
       </c>
@@ -1010,7 +1056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:15" x14ac:dyDescent="0.2">
       <c r="L17" s="2">
         <v>401113</v>
       </c>
@@ -1021,7 +1067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:15" x14ac:dyDescent="0.2">
       <c r="L18" s="3">
         <v>398936</v>
       </c>
@@ -1032,42 +1078,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:15" x14ac:dyDescent="0.2">
       <c r="L20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="12:15" x14ac:dyDescent="0.2">
       <c r="L21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="12:15" x14ac:dyDescent="0.2">
       <c r="L22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="12:15" x14ac:dyDescent="0.2">
       <c r="L23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:15" x14ac:dyDescent="0.2">
       <c r="M24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="12:15" x14ac:dyDescent="0.2">
       <c r="M25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="12:15" x14ac:dyDescent="0.2">
       <c r="N28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="12:15" x14ac:dyDescent="0.2">
       <c r="N29" t="s">
         <v>23</v>
       </c>
@@ -1075,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="12:15" x14ac:dyDescent="0.2">
       <c r="N30">
         <v>39152</v>
       </c>
@@ -1083,7 +1129,7 @@
         <v>398938</v>
       </c>
     </row>
-    <row r="31" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="12:15" x14ac:dyDescent="0.2">
       <c r="N31">
         <v>81197</v>
       </c>
@@ -1091,7 +1137,7 @@
         <v>398938</v>
       </c>
     </row>
-    <row r="32" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="12:15" x14ac:dyDescent="0.2">
       <c r="N32">
         <v>39151</v>
       </c>
@@ -1099,7 +1145,7 @@
         <v>398939</v>
       </c>
     </row>
-    <row r="33" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N33">
         <v>81196</v>
       </c>
@@ -1107,7 +1153,7 @@
         <v>398939</v>
       </c>
     </row>
-    <row r="34" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N34">
         <v>38567</v>
       </c>
@@ -1115,7 +1161,7 @@
         <v>399757</v>
       </c>
     </row>
-    <row r="35" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N35">
         <v>38569</v>
       </c>
@@ -1123,7 +1169,7 @@
         <v>400047</v>
       </c>
     </row>
-    <row r="36" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N36">
         <v>81160</v>
       </c>
@@ -1131,7 +1177,7 @@
         <v>400047</v>
       </c>
     </row>
-    <row r="37" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N37">
         <v>38573</v>
       </c>
@@ -1139,7 +1185,7 @@
         <v>403631</v>
       </c>
     </row>
-    <row r="38" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N38">
         <v>81162</v>
       </c>
@@ -1147,12 +1193,12 @@
         <v>403631</v>
       </c>
     </row>
-    <row r="39" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N40" t="s">
         <v>24</v>
       </c>
@@ -1178,7 +1224,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N41">
         <v>81664</v>
       </c>
@@ -1204,7 +1250,7 @@
         <v>100132</v>
       </c>
     </row>
-    <row r="42" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N42">
         <v>81667</v>
       </c>
@@ -1230,7 +1276,7 @@
         <v>100132</v>
       </c>
     </row>
-    <row r="43" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N43">
         <v>81668</v>
       </c>
@@ -1256,7 +1302,7 @@
         <v>100132</v>
       </c>
     </row>
-    <row r="44" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N44">
         <v>81705</v>
       </c>
@@ -1282,7 +1328,7 @@
         <v>101131</v>
       </c>
     </row>
-    <row r="45" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N45">
         <v>81706</v>
       </c>
@@ -1308,7 +1354,7 @@
         <v>101131</v>
       </c>
     </row>
-    <row r="46" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N46">
         <v>81707</v>
       </c>
@@ -1334,7 +1380,7 @@
         <v>101131</v>
       </c>
     </row>
-    <row r="47" spans="14:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N47">
         <v>85281</v>
       </c>
@@ -1376,13 +1422,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359820E0-33CF-4586-A82D-9DCED6B5334B}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1390,10 +1436,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K4" s="1"/>
     </row>
   </sheetData>
@@ -1408,7 +1454,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>